<commit_message>
most recent excel dumps
</commit_message>
<xml_diff>
--- a/EvergreenPort/Test.xlsx
+++ b/EvergreenPort/Test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Equipment Number</t>
   </si>
@@ -32,22 +32,22 @@
     <t>BOLNumber</t>
   </si>
   <si>
-    <t>EGSU9160238</t>
-  </si>
-  <si>
-    <t>EVER LYRIC</t>
-  </si>
-  <si>
-    <t>025</t>
-  </si>
-  <si>
-    <t>7075336789</t>
-  </si>
-  <si>
-    <t>082900007600</t>
-  </si>
-  <si>
-    <t>EISU9297055</t>
+    <t>FSCU8730350</t>
+  </si>
+  <si>
+    <t>EVER LISSOME</t>
+  </si>
+  <si>
+    <t>01076</t>
+  </si>
+  <si>
+    <t>DJLAXA3786864</t>
+  </si>
+  <si>
+    <t>7075333857</t>
+  </si>
+  <si>
+    <t>6198931060</t>
   </si>
   <si>
     <t>CBHU8793284</t>
@@ -56,9 +56,6 @@
     <t>EVER ELITE</t>
   </si>
   <si>
-    <t>01076</t>
-  </si>
-  <si>
     <t>7075346728</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>EMCU1432958</t>
   </si>
   <si>
-    <t>EVER LISSOME</t>
-  </si>
-  <si>
     <t>029</t>
   </si>
   <si>
@@ -92,33 +86,6 @@
     <t>061900005604</t>
   </si>
   <si>
-    <t>EGHU9212847</t>
-  </si>
-  <si>
-    <t>7075347203</t>
-  </si>
-  <si>
-    <t>EGLV082900016307</t>
-  </si>
-  <si>
-    <t>EITU1562304</t>
-  </si>
-  <si>
-    <t>7075347201</t>
-  </si>
-  <si>
-    <t>0829000162936293</t>
-  </si>
-  <si>
-    <t>TCKU6539618</t>
-  </si>
-  <si>
-    <t>7075347205</t>
-  </si>
-  <si>
-    <t>EGLV082900016285</t>
-  </si>
-  <si>
     <t>TCLU4933804</t>
   </si>
   <si>
@@ -129,6 +96,18 @@
   </si>
   <si>
     <t>TGHU8187214</t>
+  </si>
+  <si>
+    <t>BMOU4797358</t>
+  </si>
+  <si>
+    <t>DJLAXA3780305</t>
+  </si>
+  <si>
+    <t>7075342252</t>
+  </si>
+  <si>
+    <t>061900007453</t>
   </si>
 </sst>
 </file>
@@ -173,7 +152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -213,50 +192,50 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -267,16 +246,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -287,16 +266,16 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -307,16 +286,16 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -324,139 +303,79 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some python scripts + latest data
</commit_message>
<xml_diff>
--- a/EvergreenPort/Test.xlsx
+++ b/EvergreenPort/Test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Equipment Number</t>
   </si>
@@ -32,6 +32,24 @@
     <t>BOLNumber</t>
   </si>
   <si>
+    <t>TLLU4140075</t>
+  </si>
+  <si>
+    <t>TRITON</t>
+  </si>
+  <si>
+    <t>00016</t>
+  </si>
+  <si>
+    <t>DJLAXA3787663</t>
+  </si>
+  <si>
+    <t>7075348470</t>
+  </si>
+  <si>
+    <t>082900024555</t>
+  </si>
+  <si>
     <t>FSCU8730350</t>
   </si>
   <si>
@@ -84,18 +102,6 @@
   </si>
   <si>
     <t>061900005604</t>
-  </si>
-  <si>
-    <t>TCLU4933804</t>
-  </si>
-  <si>
-    <t>7075346748</t>
-  </si>
-  <si>
-    <t>149900450168</t>
-  </si>
-  <si>
-    <t>TGHU8187214</t>
   </si>
   <si>
     <t>BMOU4797358</t>
@@ -152,7 +158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -206,176 +212,156 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>